<commit_message>
Zeeman results, Bragg report
</commit_message>
<xml_diff>
--- a/Camera di Bragg/results_Bragg/resolution/Resolution.xlsx
+++ b/Camera di Bragg/results_Bragg/resolution/Resolution.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Desktop\LAB2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Desktop\LAB2020\spectroscopy-lab\Camera di Bragg\results_Bragg\resolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE69843B-775B-4F85-B17F-22D02B6CB9CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC52C895-4B7A-4307-B375-49237F1C056A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{F05BA7E4-BBFF-4399-BD31-FED43A891955}"/>
   </bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>